<commit_message>
Falta una pregunta de las justificaciones que pidio lucho
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josec\git\TPdds2020_Grupo8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA50054A-C591-4D9C-8CBE-5DF2C23057D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE20992-8790-4111-805C-8C1F451F1EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Decisión</t>
   </si>
@@ -125,9 +135,6 @@
     <t>ValidadorContraseña</t>
   </si>
   <si>
-    <t>Se eligio hacer un singleton ya que es solo unobjeto el cual se hará cargo de verificar las contraseñas.</t>
-  </si>
-  <si>
     <t>El singleton nos permite asegurar que solo un objeto es creado.</t>
   </si>
   <si>
@@ -158,9 +165,6 @@
     <t>La compra tiene un presupuesto elegido como atributo</t>
   </si>
   <si>
-    <t>Se genero un objeto que tenga toda la logica que corresponde a la validación</t>
-  </si>
-  <si>
     <t>Que la validación la haga la propia compra</t>
   </si>
   <si>
@@ -174,13 +178,43 @@
   </si>
   <si>
     <t>ENTREGA 2</t>
+  </si>
+  <si>
+    <t>Se genero un objeto que tenga toda la logica que corresponde a la validación de la operación egreso y el presupuesto.</t>
+  </si>
+  <si>
+    <t>Se eligio hacer un singleton ya que es solo un objeto SEPARADO el cual se hará cargo de verificar las contraseñas.</t>
+  </si>
+  <si>
+    <t>Que la validación de la contraseña la haga el objeto usuario.</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Este tiene una descripcion, un valor y una cantidad. Además tiene un metodo precioTotal.</t>
+  </si>
+  <si>
+    <t>Tener un obj producto y que el item sea uno o varios productos</t>
+  </si>
+  <si>
+    <t>Los items no son el objeto principal del sist. Despues el precio total va como metodo y no como atributo porque es interesante poder llamarlo.</t>
+  </si>
+  <si>
+    <t>ENTREGA 3</t>
+  </si>
+  <si>
+    <t>ENTREGA 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ¿cómo relacionan los ítems del presupuesto y la compra?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,19 +224,53 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -225,23 +293,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Celda de comprobación" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Salida" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -577,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,257 +739,321 @@
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="162" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="89.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="129.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lo que fuimos hablando
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josec\git\TPdds2020_Grupo8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8BC839-8715-4874-BBA7-226839C6EA05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737113E7-FF7B-42CF-B2A9-C2571EF7B363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Decisión</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>Simplifica la operacion y además tanto clasificacion padre e hijo harían lo mismo. (Le cambiamos el nombre de categoria a clasificacion para no repetir las de las organizaciones ya que ellas estan establecidas por AFIP y esto es algo propio del negocio.)</t>
+  </si>
+  <si>
+    <t>ENTREGA 4</t>
+  </si>
+  <si>
+    <t>Vinculador</t>
+  </si>
+  <si>
+    <t>La organización decide una sola duración para la vinculación de un ingreso.</t>
+  </si>
+  <si>
+    <t>Cada ingreso tenga su propia duración del periodo de vinculación.</t>
+  </si>
+  <si>
+    <t>Es más sencillo a la implementación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Varios egresos corresponden a un ingreso. Pero nunca un egreso va a corresponder a varios ingresos</t>
+  </si>
+  <si>
+    <t>En base al mail de Luciano Straccia "[utndds2020] Entrega 4: vinculación entre ingresos y egresos".</t>
+  </si>
+  <si>
+    <t>Que varios egresos tengan varios ingresos.</t>
   </si>
 </sst>
 </file>
@@ -433,36 +457,6 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
@@ -476,13 +470,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -506,20 +526,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="2" builtinId="23"/>
@@ -860,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1208,7 @@
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1214,37 +1237,161 @@
       <c r="E22" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="16"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E26" s="11"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
El persistance de Ignacio y puse algo en excel para justificar el commit, si no se enojan.
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josec\git\TPdds2020_Grupo8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737113E7-FF7B-42CF-B2A9-C2571EF7B363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1AA219-6983-4337-9303-BDF2151905F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
   <si>
     <t>Decisión</t>
   </si>
@@ -271,6 +271,72 @@
   </si>
   <si>
     <t>Que varios egresos tengan varios ingresos.</t>
+  </si>
+  <si>
+    <t>Persistencia</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <t>Decidimos hacer un single class ya que no se diferencian mucho los distintos proveedores.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Para que toda la informacion de TODOS los</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>proveedores estuviera junta y sea fácil de consultar.</t>
+    </r>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>EntidadJuridica y entidad base</t>
+  </si>
+  <si>
+    <t>Decidimos hacer un single class de todas las categorias.</t>
+  </si>
+  <si>
+    <t>Table per class por ejemplo o join table.</t>
+  </si>
+  <si>
+    <t>Una single table.</t>
+  </si>
+  <si>
+    <t>Hicimos una clase por cada subclase.</t>
+  </si>
+  <si>
+    <t>Para que toda la informacion de TODOS las categorias estuviera junta y sea fácil de consultar.</t>
+  </si>
+  <si>
+    <t>Al tener por separada la informacion mantenemos la seguridad de la misma, ademas que la informacion de cada subclase es muy distinta</t>
   </si>
 </sst>
 </file>
@@ -334,7 +400,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -502,7 +574,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -543,6 +615,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="2" builtinId="23"/>
@@ -885,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +971,7 @@
     <col min="5" max="5" width="129.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="66" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1303,29 +1376,63 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>

</xml_diff>

<commit_message>
2 Repos y arreglos a medias de pantallas. Revisar asociarEgryIng2
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igna\Documents\UTN Sistemas\Diseño de Sistemas\TP Anual\TPdds2020_Grupo8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josec\git\TPdds2020_Grupo8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7581CA7-BEFA-4E94-A164-689E3906558A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F70F88-EF68-49D6-93DF-951CCFF7B39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="119">
   <si>
     <t>Decisión</t>
   </si>
@@ -377,12 +377,54 @@
   <si>
     <t>Es un valor de fácil modificación aunque no aumentaría la complejidad incluirlo en alguna tabla de configuración del sistema en futuras entregas</t>
   </si>
+  <si>
+    <t>ENTREGA 5</t>
+  </si>
+  <si>
+    <t>ENTREGA 6</t>
+  </si>
+  <si>
+    <t>DEFINIR PATRON DE INTERACION</t>
+  </si>
+  <si>
+    <t>Hay una bitacora por usuario. Si este tiene proyectos asociados, podrá visualizarlos allí.</t>
+  </si>
+  <si>
+    <t>Bitacora</t>
+  </si>
+  <si>
+    <t>Que exista una unica y que permitamos a todos los usuarios acceder a toda la información.</t>
+  </si>
+  <si>
+    <t>Para mantener la seguridad de la información, más al ser un tema de dinero obtenido del estado.</t>
+  </si>
+  <si>
+    <t>Existe un proyecto, el cual será registrado en una "OperacionRegitrada" para despues ser guardada en la bitacora.</t>
+  </si>
+  <si>
+    <t>La Bitacora es el unico elemento que se relaciona con la base de datos de Mongo db</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Que toda la información este en una sola clase.</t>
+  </si>
+  <si>
+    <t>Que varias Clases interactuen con la base de datos.</t>
+  </si>
+  <si>
+    <t>Al ser la unica que interactua reducimos la posibilidad de fallas.</t>
+  </si>
+  <si>
+    <t>Menor acoplamiento.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +479,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -613,7 +662,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -655,6 +704,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="2" builtinId="23"/>
@@ -995,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z38"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="E23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1057,7 @@
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="174" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="89.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="155.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="173.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="66" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1536,14 +1586,20 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="19" t="s">
+        <v>107</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
@@ -1557,23 +1613,97 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update justificaciones de diseño
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josec\git\TPdds2020_Grupo8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F70F88-EF68-49D6-93DF-951CCFF7B39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E544A5A-3CF8-4DEC-97FB-2A02471527D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="125">
   <si>
     <t>Decisión</t>
   </si>
@@ -384,9 +384,6 @@
     <t>ENTREGA 6</t>
   </si>
   <si>
-    <t>DEFINIR PATRON DE INTERACION</t>
-  </si>
-  <si>
     <t>Hay una bitacora por usuario. Si este tiene proyectos asociados, podrá visualizarlos allí.</t>
   </si>
   <si>
@@ -418,13 +415,34 @@
   </si>
   <si>
     <t>Menor acoplamiento.</t>
+  </si>
+  <si>
+    <t>Interacción</t>
+  </si>
+  <si>
+    <t>Uso del patrón MVC para la vinculación del Backend ya creado, con la nueva interfaz gráfica requerida</t>
+  </si>
+  <si>
+    <t>Utilización de otros patrones (MVP/MVVC/etc)</t>
+  </si>
+  <si>
+    <t>Utilizando este patrón logramos una correcta separación de capas, logrando que la lógica de negocio ya creada, no se mezcle con la nueva interfaz gráfica</t>
+  </si>
+  <si>
+    <t>Utilización de Spark para aplicar el patrón MVC</t>
+  </si>
+  <si>
+    <t>Utilizar otro framework, por ej, Spring</t>
+  </si>
+  <si>
+    <t>A nivel técnico, el resultado que se alcanzaría con un Framework o el otro sería similar. Se decidió por Spark ya que consideramos el más práctico para este trabajo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,13 +497,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -704,7 +715,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Celda de comprobación" xfId="2" builtinId="23"/>
@@ -1047,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1334,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
@@ -1596,19 +1607,35 @@
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="C34" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
@@ -1624,16 +1651,16 @@
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1641,16 +1668,16 @@
         <v>8</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,16 +1685,16 @@
         <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agregada nueva decisión de diseño
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cingo\Documents\TPdds2020_Grupo8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E544A5A-3CF8-4DEC-97FB-2A02471527D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2690E700-691F-41EE-920D-7FF7789A44D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
   <si>
     <t>Decisión</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>A nivel técnico, el resultado que se alcanzaría con un Framework o el otro sería similar. Se decidió por Spark ya que consideramos el más práctico para este trabajo</t>
+  </si>
+  <si>
+    <t>Consideramos que el que crea un proyecto es su mismo director (usuario)</t>
+  </si>
+  <si>
+    <t>Que haya un campo para elegir el usuario director del nuevo proyecto</t>
+  </si>
+  <si>
+    <t>Es más sencillo.</t>
   </si>
 </sst>
 </file>
@@ -1058,20 +1067,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="174" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="173.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="173.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="66" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="66" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1088,7 +1097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
@@ -1097,7 +1106,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1146,7 +1155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1195,7 +1204,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
@@ -1268,7 +1277,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1285,7 +1294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1311,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
@@ -1351,7 +1360,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="7" t="s">
@@ -1360,7 +1369,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1394,7 +1403,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
@@ -1432,7 +1441,7 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="16" t="s">
@@ -1441,7 +1450,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -1458,7 +1467,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>80</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -1509,7 +1518,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>80</v>
       </c>
@@ -1543,7 +1552,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>80</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
@@ -1577,7 +1586,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="16" t="s">
@@ -1603,7 +1612,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1620,7 +1629,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -1637,7 +1646,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="16" t="s">
@@ -1646,7 +1655,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1663,7 +1672,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -1680,7 +1689,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -1697,35 +1706,45 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>

</xml_diff>